<commit_message>
Done for the day
Done for the day
</commit_message>
<xml_diff>
--- a/data/heat_map_bydel.xlsx
+++ b/data/heat_map_bydel.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,15 +452,20 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>neighbourhood_group</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Bydel_area</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Bydel_centroid_longitude</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Bydel_centroid_latitude</t>
         </is>
@@ -484,12 +489,15 @@
         </is>
       </c>
       <c r="E2" t="n">
+        <v>16</v>
+      </c>
+      <c r="F2" t="n">
         <v>2.662348414065196e-09</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>10.66947342625791</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>59.95442792841938</v>
       </c>
     </row>
@@ -511,12 +519,15 @@
         </is>
       </c>
       <c r="E3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" t="n">
         <v>2.534098797355098e-09</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>10.73904200385525</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>59.89658022081645</v>
       </c>
     </row>
@@ -538,12 +549,15 @@
         </is>
       </c>
       <c r="E4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" t="n">
         <v>2.201609168873283e-09</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>10.69122255053093</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>59.90899644523395</v>
       </c>
     </row>
@@ -565,12 +579,15 @@
         </is>
       </c>
       <c r="E5" t="n">
+        <v>9</v>
+      </c>
+      <c r="F5" t="n">
         <v>1.899613236245643e-09</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>10.83308507019546</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>59.89071973687254</v>
       </c>
     </row>
@@ -588,16 +605,19 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>St.Hanshaugen</t>
+          <t>St. Hanshaugen</t>
         </is>
       </c>
       <c r="E6" t="n">
+        <v>13</v>
+      </c>
+      <c r="F6" t="n">
         <v>5.742810386971385e-10</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>10.73931389921908</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>59.92880855152309</v>
       </c>
     </row>
@@ -619,12 +639,15 @@
         </is>
       </c>
       <c r="E7" t="n">
+        <v>7</v>
+      </c>
+      <c r="F7" t="n">
         <v>2.199905746902732e-09</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>10.75767426859678</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>59.954423727398</v>
       </c>
     </row>
@@ -646,12 +669,15 @@
         </is>
       </c>
       <c r="E8" t="n">
+        <v>10</v>
+      </c>
+      <c r="F8" t="n">
         <v>4.994280770493793e-10</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>10.76455557556124</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>59.93820640164834</v>
       </c>
     </row>
@@ -673,12 +699,15 @@
         </is>
       </c>
       <c r="E9" t="n">
+        <v>5</v>
+      </c>
+      <c r="F9" t="n">
         <v>7.634455628511919e-10</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>10.77760748822943</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>59.9251328295058</v>
       </c>
     </row>
@@ -700,12 +729,15 @@
         </is>
       </c>
       <c r="E10" t="n">
+        <v>11</v>
+      </c>
+      <c r="F10" t="n">
         <v>4.164492940636499e-10</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>10.74030706708456</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>59.90935192363423</v>
       </c>
     </row>
@@ -727,12 +759,15 @@
         </is>
       </c>
       <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
         <v>2.199378835616355e-09</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>10.86541004238613</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>59.92957236497114</v>
       </c>
     </row>
@@ -754,12 +789,15 @@
         </is>
       </c>
       <c r="E12" t="n">
+        <v>4</v>
+      </c>
+      <c r="F12" t="n">
         <v>1.132710732174006e-09</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>10.88318982243611</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>59.96148592393411</v>
       </c>
     </row>
@@ -781,12 +819,15 @@
         </is>
       </c>
       <c r="E13" t="n">
+        <v>14</v>
+      </c>
+      <c r="F13" t="n">
         <v>1.32601645013397e-09</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>10.92229184819139</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>59.95521809987405</v>
       </c>
     </row>
@@ -808,12 +849,15 @@
         </is>
       </c>
       <c r="E14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" t="n">
         <v>1.272830290694936e-09</v>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>10.82354344342945</v>
       </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>59.93899539231557</v>
       </c>
     </row>
@@ -835,12 +879,15 @@
         </is>
       </c>
       <c r="E15" t="n">
+        <v>15</v>
+      </c>
+      <c r="F15" t="n">
         <v>1.568443631442403e-09</v>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>10.66251587970839</v>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>59.92683094151222</v>
       </c>
     </row>
@@ -862,12 +909,15 @@
         </is>
       </c>
       <c r="E16" t="n">
+        <v>8</v>
+      </c>
+      <c r="F16" t="n">
         <v>4.268702536375804e-09</v>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
         <v>10.77890542346871</v>
       </c>
-      <c r="G16" t="n">
+      <c r="H16" t="n">
         <v>59.87074090603935</v>
       </c>
     </row>
@@ -889,12 +939,15 @@
         </is>
       </c>
       <c r="E17" t="n">
+        <v>12</v>
+      </c>
+      <c r="F17" t="n">
         <v>3.276442276151093e-09</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>10.8199084776764</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>59.83409690504696</v>
       </c>
     </row>

</xml_diff>